<commit_message>
updating image stimuli file
</commit_message>
<xml_diff>
--- a/psychopy_expt/searchDisc/image_stimuli.xlsx
+++ b/psychopy_expt/searchDisc/image_stimuli.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcin\Documents\GitHub\APP_VS\psychopy_expt\searchDisc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anna\Documents\APP_VS_git\psychopy_expt\searchDisc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C6DDD0-463E-440A-B71F-1F18D8FE3196}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC67C11-F5FB-4904-92F5-2CCB274BDEF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B5DA56B9-5FF9-4263-B0C3-36A3A7D4C8B4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B5DA56B9-5FF9-4263-B0C3-36A3A7D4C8B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1841,11 +1841,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2625AB94-AFAF-4F86-94D3-1AB2CE50B357}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A445" workbookViewId="0">
-      <selection activeCell="C384" sqref="C384"/>
+    <sheetView tabSelected="1" topLeftCell="A214" workbookViewId="0">
+      <selection activeCell="D229" sqref="D229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="47.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -3604,7 +3607,7 @@
         <v>96</v>
       </c>
       <c r="C160">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -4305,10 +4308,10 @@
         <v>227</v>
       </c>
       <c r="B224" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C224">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
@@ -6417,10 +6420,10 @@
         <v>419</v>
       </c>
       <c r="B416" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C416">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Revert "updating image stimuli file"
This reverts commit da0c62e25c299677cba59ad2fc2a101b18cb3308.
</commit_message>
<xml_diff>
--- a/psychopy_expt/searchDisc/image_stimuli.xlsx
+++ b/psychopy_expt/searchDisc/image_stimuli.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anna\Documents\APP_VS_git\psychopy_expt\searchDisc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcin\Documents\GitHub\APP_VS\psychopy_expt\searchDisc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC67C11-F5FB-4904-92F5-2CCB274BDEF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C6DDD0-463E-440A-B71F-1F18D8FE3196}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B5DA56B9-5FF9-4263-B0C3-36A3A7D4C8B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B5DA56B9-5FF9-4263-B0C3-36A3A7D4C8B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1841,14 +1841,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2625AB94-AFAF-4F86-94D3-1AB2CE50B357}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A214" workbookViewId="0">
-      <selection activeCell="D229" sqref="D229"/>
+    <sheetView tabSelected="1" topLeftCell="A445" workbookViewId="0">
+      <selection activeCell="C384" sqref="C384"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="47.85546875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -3607,7 +3604,7 @@
         <v>96</v>
       </c>
       <c r="C160">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -4308,10 +4305,10 @@
         <v>227</v>
       </c>
       <c r="B224" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C224">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
@@ -6420,10 +6417,10 @@
         <v>419</v>
       </c>
       <c r="B416" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C416">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
I'm only updating an excel file I stg
</commit_message>
<xml_diff>
--- a/psychopy_expt/searchDisc/image_stimuli.xlsx
+++ b/psychopy_expt/searchDisc/image_stimuli.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcin\Documents\GitHub\APP_VS\psychopy_expt\searchDisc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anna\Documents\APP_VS_git\psychopy_expt\searchDisc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C6DDD0-463E-440A-B71F-1F18D8FE3196}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C59256-601A-41CA-BEBC-802D13B851CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B5DA56B9-5FF9-4263-B0C3-36A3A7D4C8B4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B5DA56B9-5FF9-4263-B0C3-36A3A7D4C8B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1841,11 +1841,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2625AB94-AFAF-4F86-94D3-1AB2CE50B357}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A445" workbookViewId="0">
-      <selection activeCell="C384" sqref="C384"/>
+    <sheetView tabSelected="1" topLeftCell="A406" workbookViewId="0">
+      <selection activeCell="C418" sqref="C418"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="47.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -3604,7 +3607,7 @@
         <v>96</v>
       </c>
       <c r="C160">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -6417,10 +6420,10 @@
         <v>419</v>
       </c>
       <c r="B416" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C416">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>